<commit_message>
Merged PR 9409: Remaining
Related work items: #32796, #33759
</commit_message>
<xml_diff>
--- a/ApolloQA/Data/RatingManual/MO/UM00026.IncreasedSplitLimitFactors.xlsx
+++ b/ApolloQA/Data/RatingManual/MO/UM00026.IncreasedSplitLimitFactors.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UM00026.IncreasedSplitLimitFactors" sheetId="1" r:id="R52f44cf1f2c04203"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UM00026.IncreasedSplitLimitFactors" sheetId="1" r:id="Ree99cacb66834d36"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -838,6 +838,20 @@
     </x:row>
     <x:row>
       <x:c t="str">
+        <x:v>$500,000</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>$1,000,000</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>$10,000</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>4.4937</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
         <x:v>$1,000,000</x:v>
       </x:c>
       <x:c t="str">

</xml_diff>